<commit_message>
feat: move fbref scraper to src and add integration test
</commit_message>
<xml_diff>
--- a/notebooks/data/valencia_cf_players_2020_2024.xlsx
+++ b/notebooks/data/valencia_cf_players_2020_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,21 +469,6 @@
           <t>Contract</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Shirt Number</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Profile URL</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Photo URL</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -517,13 +502,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>/jasper-cillessen/profil/spieler/146227</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -557,13 +535,6 @@
           <t>Jul 1, 2015</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>/jaume-domenech/profil/spieler/227805</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -597,13 +568,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>/cristian-rivero/profil/spieler/398131</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -633,13 +597,6 @@
         <v>2020</v>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>/unai-etxebarria/profil/spieler/288376</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -673,13 +630,6 @@
           <t>Aug 18, 2017</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>/gabriel-paulista/profil/spieler/149498</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -713,13 +663,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>/mouctar-diakhaby/profil/spieler/346289</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -753,13 +696,6 @@
           <t>Jan 31, 2021</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>/ferro/profil/spieler/294321</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -793,13 +729,6 @@
           <t>Aug 12, 2019</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>/eliaquim-mangala/profil/spieler/90681</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -833,13 +762,6 @@
           <t>Jul 23, 2018</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>/cristiano-piccini/profil/spieler/163086</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -869,13 +791,6 @@
         <v>2020</v>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>/guillem-molina/profil/spieler/602156</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -905,13 +820,6 @@
         <v>2020</v>
       </c>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>/kevin-sibille/profil/spieler/409273</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -945,13 +853,6 @@
           <t>Jul 1, 2014</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>/jose-gaya/profil/spieler/221322</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -985,13 +886,6 @@
           <t>Jul 1, 2017</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>/toni-lato/profil/spieler/320271</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1025,13 +919,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>/alex-centelles/profil/spieler/423443</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1065,13 +952,6 @@
           <t>Jan 1, 2022</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>/jesus-vazquez/profil/spieler/623024</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1105,13 +985,6 @@
           <t>Sep 2, 2019</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>/thierry-correia/profil/spieler/367466</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1145,13 +1018,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>/geoffrey-kondogbia/profil/spieler/127189</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1185,13 +1051,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>/uros-racic/profil/spieler/417575</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1225,13 +1084,6 @@
           <t>Jul 1, 2020</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>/hugo-guillamon/profil/spieler/495629</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1265,13 +1117,6 @@
           <t>Feb 1, 2021</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>/christian-oliva/profil/spieler/563812</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1305,13 +1150,6 @@
           <t>Jan 1, 2017</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>/carlos-soler/profil/spieler/372246</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1345,13 +1183,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>/yunus-musah/profil/spieler/503991</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1385,13 +1216,6 @@
           <t>Jul 10, 2018</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>/daniel-wass/profil/spieler/63463</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1425,13 +1249,6 @@
           <t>Jan 31, 2022</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>/koba-koindredi/profil/spieler/569375</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1461,13 +1278,6 @@
         <v>2020</v>
       </c>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>/vicente-esquerdo/profil/spieler/599263</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1501,13 +1311,6 @@
           <t>Aug 27, 2018</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>/goncalo-guedes/profil/spieler/225122</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1541,13 +1344,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>/denis-cheryshev/profil/spieler/98322</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1581,13 +1377,6 @@
           <t>Jan 30, 2019</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>/alex-blanco/profil/spieler/328914</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1621,13 +1410,6 @@
           <t>Jan 30, 2019</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>/kang-in-lee/profil/spieler/557149</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1661,13 +1443,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>/jason/profil/spieler/263860</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1701,13 +1476,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>/manu-vallejo/profil/spieler/527350</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1741,13 +1509,6 @@
           <t>Jul 14, 2019</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>/maxi-gomez/profil/spieler/396894</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1781,13 +1542,6 @@
           <t>Jan 31, 2021</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>/patrick-cutrone/profil/spieler/265078</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1821,13 +1575,6 @@
           <t>Aug 12, 2018</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>/kevin-gameiro/profil/spieler/27389</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1861,13 +1608,6 @@
           <t>Jan 31, 2019</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>/ruben-sobrino/profil/spieler/85383</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1901,13 +1641,6 @@
           <t>Aug 28, 2024</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>/giorgi-mamardashvili/profil/spieler/502676</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1941,13 +1674,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>/jasper-cillessen/profil/spieler/146227</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1981,13 +1707,6 @@
           <t>Jul 1, 2015</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>/jaume-domenech/profil/spieler/227805</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2021,13 +1740,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>/cristian-rivero/profil/spieler/398131</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2057,13 +1769,6 @@
         <v>2021</v>
       </c>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>/charlie-perez/profil/spieler/707271</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2097,13 +1802,6 @@
           <t>Jul 12, 2021</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>/omar-alderete/profil/spieler/353032</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2137,13 +1835,6 @@
           <t>Aug 18, 2017</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>/gabriel-paulista/profil/spieler/149498</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2177,13 +1868,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>/mouctar-diakhaby/profil/spieler/346289</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2217,13 +1901,6 @@
           <t>Jan 25, 2022</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>/eray-comert/profil/spieler/298583</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2257,13 +1934,6 @@
           <t>Jul 23, 2018</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>/cristiano-piccini/profil/spieler/163086</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2297,13 +1967,6 @@
           <t>Jan 1, 2023</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>/cristhian-mosquera/profil/spieler/646750</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2337,13 +2000,6 @@
           <t>Jan 18, 2024</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>/cesar-tarrega/profil/spieler/707274</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2373,13 +2029,6 @@
         <v>2021</v>
       </c>
       <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>/ruben-iranzo/profil/spieler/668212</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2413,13 +2062,6 @@
           <t>Jul 1, 2014</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>/jose-gaya/profil/spieler/221322</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2453,13 +2095,6 @@
           <t>Jan 1, 2022</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>/jesus-vazquez/profil/spieler/623024</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2493,13 +2128,6 @@
           <t>Jul 1, 2017</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>/toni-lato/profil/spieler/320271</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2533,13 +2161,6 @@
           <t>Sep 2, 2019</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>/thierry-correia/profil/spieler/367466</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2573,13 +2194,6 @@
           <t>Aug 30, 2021</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>/dimitri-foulquier/profil/spieler/170472</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2609,13 +2223,6 @@
         <v>2021</v>
       </c>
       <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>/joseda-menargues/profil/spieler/589459</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2649,13 +2256,6 @@
           <t>Jul 1, 2020</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>/hugo-guillamon/profil/spieler/495629</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2689,13 +2289,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>/uros-racic/profil/spieler/417575</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2729,13 +2322,6 @@
           <t>Jan 1, 2017</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>/carlos-soler/profil/spieler/372246</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2769,13 +2355,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>/yunus-musah/profil/spieler/503991</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2809,13 +2388,6 @@
           <t>Sep 1, 2022</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>/ilaix-moriba/profil/spieler/617074</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2849,13 +2421,6 @@
           <t>Jul 10, 2018</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>/daniel-wass/profil/spieler/63463</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2889,13 +2454,6 @@
           <t>Jan 31, 2022</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>/koba-koindredi/profil/spieler/569375</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2929,13 +2487,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>/javi-guerra/profil/spieler/834764</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2965,13 +2516,6 @@
         <v>2021</v>
       </c>
       <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>/lass-sangare/profil/spieler/944124</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3001,13 +2545,6 @@
         <v>2021</v>
       </c>
       <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>/yellu-santiago/profil/spieler/941869</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3037,13 +2574,6 @@
         <v>2021</v>
       </c>
       <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>/pedro-aleman/profil/spieler/699771</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3077,13 +2607,6 @@
           <t>Aug 27, 2018</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>/goncalo-guedes/profil/spieler/225122</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3117,13 +2640,6 @@
           <t>Jan 31, 2022</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>/bryan-gil/profil/spieler/537382</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3157,13 +2673,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>/denis-cheryshev/profil/spieler/98322</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3197,13 +2706,6 @@
           <t>Jan 30, 2019</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>/alex-blanco/profil/spieler/328914</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3237,13 +2739,6 @@
           <t>Aug 31, 2021</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>/helder-costa/profil/spieler/173900</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3277,13 +2772,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>/jason/profil/spieler/263860</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3317,13 +2805,6 @@
           <t>Jul 1, 2024</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>/hugo-gonzalez/profil/spieler/707279</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3357,13 +2838,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>/diego-lopez/profil/spieler/617081</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3397,13 +2871,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>/manu-vallejo/profil/spieler/527350</t>
-        </is>
-      </c>
-      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3437,13 +2904,6 @@
           <t>Jul 14, 2019</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>/maxi-gomez/profil/spieler/396894</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3477,13 +2937,6 @@
           <t>Jul 1, 2022</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>/hugo-duro/profil/spieler/573775</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3517,13 +2970,6 @@
           <t>Aug 25, 2021</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>/marcos-andre/profil/spieler/481084</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3557,13 +3003,6 @@
           <t>Jan 31, 2019</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>/ruben-sobrino/profil/spieler/85383</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3593,13 +3032,6 @@
         <v>2021</v>
       </c>
       <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>/mario-dominguez/profil/spieler/941867</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3633,13 +3065,6 @@
           <t>Aug 28, 2024</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>/giorgi-mamardashvili/profil/spieler/502676</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3673,13 +3098,6 @@
           <t>Jul 1, 2015</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>/jaume-domenech/profil/spieler/227805</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3713,13 +3131,6 @@
           <t>Sep 28, 2022</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>/iago-herrerin/profil/spieler/71570</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3749,13 +3160,6 @@
         <v>2022</v>
       </c>
       <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>/emilio-bernad/profil/spieler/480966</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3789,13 +3193,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>/cristian-rivero/profil/spieler/398131</t>
-        </is>
-      </c>
-      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3825,13 +3222,6 @@
         <v>2022</v>
       </c>
       <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>/charlie-perez/profil/spieler/707271</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3865,13 +3255,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr"/>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>/mouctar-diakhaby/profil/spieler/346289</t>
-        </is>
-      </c>
-      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3905,13 +3288,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>/cenk-ozkacar/profil/spieler/615350</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3945,13 +3321,6 @@
           <t>Jan 25, 2022</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>/eray-comert/profil/spieler/298583</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3985,13 +3354,6 @@
           <t>Aug 18, 2017</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>/gabriel-paulista/profil/spieler/149498</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4025,13 +3387,6 @@
           <t>Jan 1, 2023</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>/cristhian-mosquera/profil/spieler/646750</t>
-        </is>
-      </c>
-      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4061,13 +3416,6 @@
         <v>2022</v>
       </c>
       <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>/ruben-iranzo/profil/spieler/668212</t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4101,13 +3449,6 @@
           <t>Jul 1, 2014</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>/jose-gaya/profil/spieler/221322</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4141,13 +3482,6 @@
           <t>Jan 1, 2022</t>
         </is>
       </c>
-      <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>/jesus-vazquez/profil/spieler/623024</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4181,13 +3515,6 @@
           <t>Jul 1, 2017</t>
         </is>
       </c>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>/toni-lato/profil/spieler/320271</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4221,13 +3548,6 @@
           <t>Sep 2, 2019</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>/thierry-correia/profil/spieler/367466</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4261,13 +3581,6 @@
           <t>Aug 30, 2021</t>
         </is>
       </c>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>/dimitri-foulquier/profil/spieler/170472</t>
-        </is>
-      </c>
-      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4301,13 +3614,6 @@
           <t>Jul 1, 2020</t>
         </is>
       </c>
-      <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>/hugo-guillamon/profil/spieler/495629</t>
-        </is>
-      </c>
-      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4341,13 +3647,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>/uros-racic/profil/spieler/417575</t>
-        </is>
-      </c>
-      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4381,13 +3680,6 @@
           <t>Jan 1, 2017</t>
         </is>
       </c>
-      <c r="H100" t="inlineStr"/>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>/carlos-soler/profil/spieler/372246</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4421,13 +3713,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>/yunus-musah/profil/spieler/503991</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4461,13 +3746,6 @@
           <t>Aug 13, 2022</t>
         </is>
       </c>
-      <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>/nico-gonzalez/profil/spieler/466805</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4501,13 +3779,6 @@
           <t>Sep 1, 2022</t>
         </is>
       </c>
-      <c r="H103" t="inlineStr"/>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>/ilaix-moriba/profil/spieler/617074</t>
-        </is>
-      </c>
-      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4541,13 +3812,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>/javi-guerra/profil/spieler/834764</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4581,13 +3845,6 @@
           <t>Jan 31, 2022</t>
         </is>
       </c>
-      <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>/koba-koindredi/profil/spieler/569375</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4617,13 +3874,6 @@
         <v>2022</v>
       </c>
       <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>/tiago-ribeiro/profil/spieler/504084</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4653,13 +3903,6 @@
         <v>2022</v>
       </c>
       <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>/yellu-santiago/profil/spieler/941869</t>
-        </is>
-      </c>
-      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4693,13 +3936,6 @@
           <t>Aug 25, 2022</t>
         </is>
       </c>
-      <c r="H108" t="inlineStr"/>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>/andre-almeida/profil/spieler/375382</t>
-        </is>
-      </c>
-      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4733,13 +3969,6 @@
           <t>Sep 1, 2022</t>
         </is>
       </c>
-      <c r="H109" t="inlineStr"/>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>/justin-kluivert/profil/spieler/330659</t>
-        </is>
-      </c>
-      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4773,13 +4002,6 @@
           <t>Jul 28, 2022</t>
         </is>
       </c>
-      <c r="H110" t="inlineStr"/>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>/samuel-lino/profil/spieler/694928</t>
-        </is>
-      </c>
-      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4813,13 +4035,6 @@
           <t>Jul 12, 2022</t>
         </is>
       </c>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>/samu-castillejo/profil/spieler/195171</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4853,13 +4068,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>/diego-lopez/profil/spieler/617081</t>
-        </is>
-      </c>
-      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4893,13 +4101,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H113" t="inlineStr"/>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>/fran-perez/profil/spieler/622988</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4933,13 +4134,6 @@
           <t>Jul 1, 2019</t>
         </is>
       </c>
-      <c r="H114" t="inlineStr"/>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>/manu-vallejo/profil/spieler/527350</t>
-        </is>
-      </c>
-      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4973,13 +4167,6 @@
           <t>Jul 14, 2019</t>
         </is>
       </c>
-      <c r="H115" t="inlineStr"/>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>/maxi-gomez/profil/spieler/396894</t>
-        </is>
-      </c>
-      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5013,13 +4200,6 @@
           <t>Jul 1, 2022</t>
         </is>
       </c>
-      <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>/hugo-duro/profil/spieler/573775</t>
-        </is>
-      </c>
-      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5053,13 +4233,6 @@
           <t>Aug 29, 2022</t>
         </is>
       </c>
-      <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>/edinson-cavani/profil/spieler/48280</t>
-        </is>
-      </c>
-      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5093,13 +4266,6 @@
           <t>Aug 25, 2021</t>
         </is>
       </c>
-      <c r="H118" t="inlineStr"/>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>/marcos-andre/profil/spieler/481084</t>
-        </is>
-      </c>
-      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5133,13 +4299,6 @@
           <t>Jul 26, 2023</t>
         </is>
       </c>
-      <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>/alberto-mari/profil/spieler/634105</t>
-        </is>
-      </c>
-      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5169,13 +4328,6 @@
         <v>2022</v>
       </c>
       <c r="G120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>/mario-dominguez/profil/spieler/941867</t>
-        </is>
-      </c>
-      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5209,13 +4361,6 @@
           <t>Aug 28, 2024</t>
         </is>
       </c>
-      <c r="H121" t="inlineStr"/>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>/giorgi-mamardashvili/profil/spieler/502676</t>
-        </is>
-      </c>
-      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5249,13 +4394,6 @@
           <t>Jul 1, 2015</t>
         </is>
       </c>
-      <c r="H122" t="inlineStr"/>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>/jaume-domenech/profil/spieler/227805</t>
-        </is>
-      </c>
-      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5289,13 +4427,6 @@
           <t>Aug 1, 2020</t>
         </is>
       </c>
-      <c r="H123" t="inlineStr"/>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>/cristian-rivero/profil/spieler/398131</t>
-        </is>
-      </c>
-      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5325,13 +4456,6 @@
         <v>2023</v>
       </c>
       <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>/vicent-abril/profil/spieler/741251</t>
-        </is>
-      </c>
-      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5365,13 +4489,6 @@
           <t>Jan 1, 2023</t>
         </is>
       </c>
-      <c r="H125" t="inlineStr"/>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>/cristhian-mosquera/profil/spieler/646750</t>
-        </is>
-      </c>
-      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5405,13 +4522,6 @@
           <t>Oct 1, 2023</t>
         </is>
       </c>
-      <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>/yarek-gasiorowski/profil/spieler/895334</t>
-        </is>
-      </c>
-      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5445,13 +4555,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H127" t="inlineStr"/>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>/cenk-ozkacar/profil/spieler/615350</t>
-        </is>
-      </c>
-      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5485,13 +4588,6 @@
           <t>Jul 1, 2018</t>
         </is>
       </c>
-      <c r="H128" t="inlineStr"/>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>/mouctar-diakhaby/profil/spieler/346289</t>
-        </is>
-      </c>
-      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5525,13 +4621,6 @@
           <t>Aug 18, 2017</t>
         </is>
       </c>
-      <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>/gabriel-paulista/profil/spieler/149498</t>
-        </is>
-      </c>
-      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5565,13 +4654,6 @@
           <t>Jan 18, 2024</t>
         </is>
       </c>
-      <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>/cesar-tarrega/profil/spieler/707274</t>
-        </is>
-      </c>
-      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5601,13 +4683,6 @@
         <v>2023</v>
       </c>
       <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>/ruben-iranzo/profil/spieler/668212</t>
-        </is>
-      </c>
-      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5641,13 +4716,6 @@
           <t>Jul 1, 2014</t>
         </is>
       </c>
-      <c r="H132" t="inlineStr"/>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>/jose-gaya/profil/spieler/221322</t>
-        </is>
-      </c>
-      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5681,13 +4749,6 @@
           <t>Jan 1, 2022</t>
         </is>
       </c>
-      <c r="H133" t="inlineStr"/>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>/jesus-vazquez/profil/spieler/623024</t>
-        </is>
-      </c>
-      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5721,13 +4782,6 @@
           <t>Sep 2, 2019</t>
         </is>
       </c>
-      <c r="H134" t="inlineStr"/>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>/thierry-correia/profil/spieler/367466</t>
-        </is>
-      </c>
-      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5761,13 +4815,6 @@
           <t>Aug 30, 2021</t>
         </is>
       </c>
-      <c r="H135" t="inlineStr"/>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>/dimitri-foulquier/profil/spieler/170472</t>
-        </is>
-      </c>
-      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5801,13 +4848,6 @@
           <t>Jul 8, 2023</t>
         </is>
       </c>
-      <c r="H136" t="inlineStr"/>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>/pepelu/profil/spieler/328480</t>
-        </is>
-      </c>
-      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5841,13 +4881,6 @@
           <t>Jul 1, 2020</t>
         </is>
       </c>
-      <c r="H137" t="inlineStr"/>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>/hugo-guillamon/profil/spieler/495629</t>
-        </is>
-      </c>
-      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5881,13 +4914,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H138" t="inlineStr"/>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>/javi-guerra/profil/spieler/834764</t>
-        </is>
-      </c>
-      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5917,13 +4943,6 @@
         <v>2023</v>
       </c>
       <c r="G139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>/ali-fadal/profil/spieler/980242</t>
-        </is>
-      </c>
-      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5953,13 +4972,6 @@
         <v>2023</v>
       </c>
       <c r="G140" t="inlineStr"/>
-      <c r="H140" t="inlineStr"/>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>/javi-navarro/profil/spieler/646743</t>
-        </is>
-      </c>
-      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5993,13 +5005,6 @@
           <t>Aug 25, 2022</t>
         </is>
       </c>
-      <c r="H141" t="inlineStr"/>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>/andre-almeida/profil/spieler/375382</t>
-        </is>
-      </c>
-      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6033,13 +5038,6 @@
           <t>Aug 29, 2023</t>
         </is>
       </c>
-      <c r="H142" t="inlineStr"/>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>/selim-amallah/profil/spieler/377219</t>
-        </is>
-      </c>
-      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6069,13 +5067,6 @@
         <v>2023</v>
       </c>
       <c r="G143" t="inlineStr"/>
-      <c r="H143" t="inlineStr"/>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>/pablo-gozalbez/profil/spieler/622992</t>
-        </is>
-      </c>
-      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6105,13 +5096,6 @@
         <v>2023</v>
       </c>
       <c r="G144" t="inlineStr"/>
-      <c r="H144" t="inlineStr"/>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>/martin-tejon/profil/spieler/941883</t>
-        </is>
-      </c>
-      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6145,13 +5129,6 @@
           <t>Aug 20, 2023</t>
         </is>
       </c>
-      <c r="H145" t="inlineStr"/>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>/sergi-canos/profil/spieler/251845</t>
-        </is>
-      </c>
-      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6181,13 +5158,6 @@
         <v>2023</v>
       </c>
       <c r="G146" t="inlineStr"/>
-      <c r="H146" t="inlineStr"/>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>/marco-camus/profil/spieler/636119</t>
-        </is>
-      </c>
-      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6221,13 +5191,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H147" t="inlineStr"/>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>/diego-lopez/profil/spieler/617081</t>
-        </is>
-      </c>
-      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6261,13 +5224,6 @@
           <t>Jul 1, 2023</t>
         </is>
       </c>
-      <c r="H148" t="inlineStr"/>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>/fran-perez/profil/spieler/622988</t>
-        </is>
-      </c>
-      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -6301,13 +5257,6 @@
           <t>Jan 31, 2024</t>
         </is>
       </c>
-      <c r="H149" t="inlineStr"/>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>/peter-federico/profil/spieler/710004</t>
-        </is>
-      </c>
-      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -6337,13 +5286,6 @@
         <v>2023</v>
       </c>
       <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>/david-otorbi/profil/spieler/1009766</t>
-        </is>
-      </c>
-      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6377,13 +5319,6 @@
           <t>Jul 1, 2024</t>
         </is>
       </c>
-      <c r="H151" t="inlineStr"/>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>/hugo-gonzalez/profil/spieler/707279</t>
-        </is>
-      </c>
-      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6417,13 +5352,6 @@
           <t>Jul 1, 2022</t>
         </is>
       </c>
-      <c r="H152" t="inlineStr"/>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>/hugo-duro/profil/spieler/573775</t>
-        </is>
-      </c>
-      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6457,13 +5385,6 @@
           <t>Sep 1, 2023</t>
         </is>
       </c>
-      <c r="H153" t="inlineStr"/>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>/roman-yaremchuk/profil/spieler/221958</t>
-        </is>
-      </c>
-      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6497,13 +5418,6 @@
           <t>Jul 26, 2023</t>
         </is>
       </c>
-      <c r="H154" t="inlineStr"/>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>/alberto-mari/profil/spieler/634105</t>
-        </is>
-      </c>
-      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6533,13 +5447,6 @@
         <v>2023</v>
       </c>
       <c r="G155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>/mario-dominguez/profil/spieler/941867</t>
-        </is>
-      </c>
-      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6569,13 +5476,6 @@
         <v>2023</v>
       </c>
       <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>/joselu-perez/profil/spieler/1000135</t>
-        </is>
-      </c>
-      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -6609,13 +5509,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H157" t="inlineStr"/>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>/giorgi-mamardashvili/profil/spieler/502676</t>
-        </is>
-      </c>
-      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6649,13 +5542,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H158" t="inlineStr"/>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>/stole-dimitrievski/profil/spieler/165467</t>
-        </is>
-      </c>
-      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6689,13 +5575,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H159" t="inlineStr"/>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>/jaume-domenech/profil/spieler/227805</t>
-        </is>
-      </c>
-      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -6729,13 +5608,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H160" t="inlineStr"/>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>/cristhian-mosquera/profil/spieler/646750</t>
-        </is>
-      </c>
-      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6769,13 +5641,6 @@
           <t>Jun 30, 2028</t>
         </is>
       </c>
-      <c r="H161" t="inlineStr"/>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>/cesar-tarrega/profil/spieler/707274</t>
-        </is>
-      </c>
-      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6809,13 +5674,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H162" t="inlineStr"/>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>/yarek-gasiorowski/profil/spieler/895334</t>
-        </is>
-      </c>
-      <c r="J162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6849,13 +5707,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H163" t="inlineStr"/>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>/mouctar-diakhaby/profil/spieler/346289</t>
-        </is>
-      </c>
-      <c r="J163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6889,13 +5740,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H164" t="inlineStr"/>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>/jose-gaya/profil/spieler/221322</t>
-        </is>
-      </c>
-      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6929,13 +5773,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H165" t="inlineStr"/>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>/jesus-vazquez/profil/spieler/623024</t>
-        </is>
-      </c>
-      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6969,13 +5806,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>/max-aarons/profil/spieler/471690</t>
-        </is>
-      </c>
-      <c r="J166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -7009,13 +5839,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H167" t="inlineStr"/>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>/thierry-correia/profil/spieler/367466</t>
-        </is>
-      </c>
-      <c r="J167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -7049,13 +5872,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H168" t="inlineStr"/>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>/dimitri-foulquier/profil/spieler/170472</t>
-        </is>
-      </c>
-      <c r="J168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -7089,13 +5905,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H169" t="inlineStr"/>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>/enzo-barrenechea/profil/spieler/671915</t>
-        </is>
-      </c>
-      <c r="J169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -7129,13 +5938,6 @@
           <t>Jun 30, 2028</t>
         </is>
       </c>
-      <c r="H170" t="inlineStr"/>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>/pepelu/profil/spieler/328480</t>
-        </is>
-      </c>
-      <c r="J170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -7169,13 +5971,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H171" t="inlineStr"/>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>/hugo-guillamon/profil/spieler/495629</t>
-        </is>
-      </c>
-      <c r="J171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -7209,13 +6004,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H172" t="inlineStr"/>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>/javi-guerra/profil/spieler/834764</t>
-        </is>
-      </c>
-      <c r="J172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -7249,13 +6037,6 @@
           <t>Jun 30, 2028</t>
         </is>
       </c>
-      <c r="H173" t="inlineStr"/>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t>/andre-almeida/profil/spieler/375382</t>
-        </is>
-      </c>
-      <c r="J173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7289,13 +6070,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H174" t="inlineStr"/>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>/ivan-jaime/profil/spieler/610335</t>
-        </is>
-      </c>
-      <c r="J174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -7329,13 +6103,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H175" t="inlineStr"/>
-      <c r="I175" t="inlineStr">
-        <is>
-          <t>/martin-tejon/profil/spieler/941883</t>
-        </is>
-      </c>
-      <c r="J175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7369,13 +6136,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H176" t="inlineStr"/>
-      <c r="I176" t="inlineStr">
-        <is>
-          <t>/luis-rioja/profil/spieler/278837</t>
-        </is>
-      </c>
-      <c r="J176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -7409,13 +6169,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H177" t="inlineStr"/>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>/sergi-canos/profil/spieler/251845</t>
-        </is>
-      </c>
-      <c r="J177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7449,13 +6202,6 @@
           <t>Jun 30, 2027</t>
         </is>
       </c>
-      <c r="H178" t="inlineStr"/>
-      <c r="I178" t="inlineStr">
-        <is>
-          <t>/diego-lopez/profil/spieler/617081</t>
-        </is>
-      </c>
-      <c r="J178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7489,13 +6235,6 @@
           <t>Jun 30, 2026</t>
         </is>
       </c>
-      <c r="H179" t="inlineStr"/>
-      <c r="I179" t="inlineStr">
-        <is>
-          <t>/fran-perez/profil/spieler/622988</t>
-        </is>
-      </c>
-      <c r="J179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7529,13 +6268,6 @@
           <t>Jun 30, 2028</t>
         </is>
       </c>
-      <c r="H180" t="inlineStr"/>
-      <c r="I180" t="inlineStr">
-        <is>
-          <t>/hugo-duro/profil/spieler/573775</t>
-        </is>
-      </c>
-      <c r="J180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -7569,13 +6301,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H181" t="inlineStr"/>
-      <c r="I181" t="inlineStr">
-        <is>
-          <t>/umar-sadiq/profil/spieler/337715</t>
-        </is>
-      </c>
-      <c r="J181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7609,13 +6334,6 @@
           <t>Jun 30, 2025</t>
         </is>
       </c>
-      <c r="H182" t="inlineStr"/>
-      <c r="I182" t="inlineStr">
-        <is>
-          <t>/rafa-mir/profil/spieler/361254</t>
-        </is>
-      </c>
-      <c r="J182" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>